<commit_message>
Update Inventario de variables.xlsx
</commit_message>
<xml_diff>
--- a/Inferencia_causal/Panel de datos/Inventario de variables.xlsx
+++ b/Inferencia_causal/Panel de datos/Inventario de variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP-Laptop\OneDrive - Universidad de Antioquia\Maestría en Economía\Evaluación de impacto\Inferencia-Causal\Inferencia_causal\Panel de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4D68C24-479F-428D-8089-DC0162F99D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE5E681-68EE-414E-A54D-5564C13F03C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FD8500B0-8B60-428F-9AE2-6C7D431BCC40}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FD8500B0-8B60-428F-9AE2-6C7D431BCC40}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventario variables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
   <si>
     <t>Variables</t>
   </si>
@@ -210,13 +210,172 @@
   </si>
   <si>
     <t>Número de hogares en cada comuna (suma factor hogares)</t>
+  </si>
+  <si>
+    <t>p_006</t>
+  </si>
+  <si>
+    <t>creada</t>
+  </si>
+  <si>
+    <t>p_017</t>
+  </si>
+  <si>
+    <t>p_020</t>
+  </si>
+  <si>
+    <t>p_023</t>
+  </si>
+  <si>
+    <t>p_015</t>
+  </si>
+  <si>
+    <t>p_254/12</t>
+  </si>
+  <si>
+    <t>p_045</t>
+  </si>
+  <si>
+    <t>p_035</t>
+  </si>
+  <si>
+    <t>p_058</t>
+  </si>
+  <si>
+    <t>p_066</t>
+  </si>
+  <si>
+    <t>p_076</t>
+  </si>
+  <si>
+    <t>p_308</t>
+  </si>
+  <si>
+    <t>p_307</t>
+  </si>
+  <si>
+    <t>p_018</t>
+  </si>
+  <si>
+    <t>edad&lt;18</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>idVivienda&amp;hogar</t>
+  </si>
+  <si>
+    <t>idHogar&amp;persona</t>
+  </si>
+  <si>
+    <t>FEH</t>
+  </si>
+  <si>
+    <t>P_006</t>
+  </si>
+  <si>
+    <t>P_023</t>
+  </si>
+  <si>
+    <t>P_308</t>
+  </si>
+  <si>
+    <t>P_307</t>
+  </si>
+  <si>
+    <t>P_018</t>
+  </si>
+  <si>
+    <t>P_269 (gasto)</t>
+  </si>
+  <si>
+    <t>P_016</t>
+  </si>
+  <si>
+    <t>P_022</t>
+  </si>
+  <si>
+    <t>P_049</t>
+  </si>
+  <si>
+    <t>P_039</t>
+  </si>
+  <si>
+    <t>P_064</t>
+  </si>
+  <si>
+    <t>P_074</t>
+  </si>
+  <si>
+    <t>P_077</t>
+  </si>
+  <si>
+    <t>P_073_c</t>
+  </si>
+  <si>
+    <t>P_073_b</t>
+  </si>
+  <si>
+    <t>P_021</t>
+  </si>
+  <si>
+    <t>NoForm</t>
+  </si>
+  <si>
+    <t>idVivienda&amp;sHogar</t>
+  </si>
+  <si>
+    <t>P_6</t>
+  </si>
+  <si>
+    <t>P_244</t>
+  </si>
+  <si>
+    <t>P_17</t>
+  </si>
+  <si>
+    <t>P_20</t>
+  </si>
+  <si>
+    <t>P_23</t>
+  </si>
+  <si>
+    <t>P_45</t>
+  </si>
+  <si>
+    <t>P_58</t>
+  </si>
+  <si>
+    <t>P_66</t>
+  </si>
+  <si>
+    <t>P_15</t>
+  </si>
+  <si>
+    <t>P_35</t>
+  </si>
+  <si>
+    <t>P_69</t>
+  </si>
+  <si>
+    <t>P_18</t>
+  </si>
+  <si>
+    <t>idVivienda&amp;Hogar</t>
+  </si>
+  <si>
+    <t>idHogar&amp;Orden</t>
+  </si>
+  <si>
+    <t>FEVH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +390,17 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -271,16 +441,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Variables" xfId="1" xr:uid="{3187150C-2211-4EEE-AD2D-A5BE885BC16B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,9 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F9DF53-3100-498B-B412-240E76160DD9}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -734,10 +907,16 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="P2">
         <v>1</v>
       </c>
@@ -760,10 +939,16 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="P3">
         <v>2</v>
       </c>
@@ -786,10 +971,16 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="P4">
         <v>3</v>
       </c>
@@ -812,10 +1003,16 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="P5">
         <v>4</v>
       </c>
@@ -838,10 +1035,16 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="P6">
         <v>5</v>
       </c>
@@ -864,10 +1067,16 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="P7">
         <v>1</v>
       </c>
@@ -890,10 +1099,16 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="M8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="P8">
         <v>2</v>
       </c>
@@ -916,10 +1131,16 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="P9">
         <v>3</v>
       </c>
@@ -942,10 +1163,16 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="P10">
         <v>4</v>
       </c>
@@ -968,10 +1195,16 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="M11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="P11">
         <v>5</v>
       </c>
@@ -994,10 +1227,16 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1014,10 +1253,16 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="M13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1034,10 +1279,16 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="M14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1054,10 +1305,16 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1074,10 +1331,16 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1094,10 +1357,16 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1114,10 +1383,16 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1134,10 +1409,16 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+      <c r="M19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1154,10 +1435,16 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="M20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1174,10 +1461,16 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>